<commit_message>
Added questionnaire to the app
</commit_message>
<xml_diff>
--- a/Persona-Product-Matrix.xlsx
+++ b/Persona-Product-Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deutschebank-my.sharepoint.com/personal/anand-mahendra_mehta_db_com/Documents/Hackathon2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bb8175d7e0b9cbf/Documents/Chatbot_Unnati/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E0F69A2-E7EB-4CDA-92D6-2AF9B840DAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{5E0F69A2-E7EB-4CDA-92D6-2AF9B840DAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCB63FE2-FEEA-4956-84E9-DFB1FA772182}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4884D8A7-0253-4FEB-9B67-96A3EAB68932}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4884D8A7-0253-4FEB-9B67-96A3EAB68932}"/>
   </bookViews>
   <sheets>
     <sheet name="HIgh level summary " sheetId="1" r:id="rId1"/>
@@ -488,15 +488,6 @@
     <t>Less than 50k</t>
   </si>
   <si>
-    <t>50-1l</t>
-  </si>
-  <si>
-    <t>1l-3l</t>
-  </si>
-  <si>
-    <t>3l &amp; above</t>
-  </si>
-  <si>
     <t>How secure do you feel are your current &amp; future income sources? (E.g. Salary, Business Income)</t>
   </si>
   <si>
@@ -585,13 +576,22 @@
   </si>
   <si>
     <t xml:space="preserve">Response </t>
+  </si>
+  <si>
+    <t>50k-1L</t>
+  </si>
+  <si>
+    <t>1L-3L</t>
+  </si>
+  <si>
+    <t>3L &amp; above</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1610,11 +1610,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203A8789-3A94-4B84-B234-D393C1764329}">
   <dimension ref="A1:M152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="88.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="4" customWidth="1"/>
@@ -1628,7 +1628,7 @@
     <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1682,7 +1682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>13</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="20" customFormat="1">
+    <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="20" customFormat="1">
+    <row r="5" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>18</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="20" customFormat="1">
+    <row r="6" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>24</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="20" customFormat="1">
+    <row r="8" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>16</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="20" customFormat="1">
+    <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>18</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="20" customFormat="1">
+    <row r="10" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>21</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="20" customFormat="1">
+    <row r="12" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="20" customFormat="1">
+    <row r="13" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>18</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="20" customFormat="1">
+    <row r="14" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>29</v>
       </c>
@@ -2077,67 +2077,67 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="13"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="13"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="11"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="11"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="9"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>36</v>
       </c>
@@ -2145,47 +2145,47 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
       <c r="B34" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>42</v>
       </c>
@@ -2193,42 +2193,42 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="14" customFormat="1">
+    <row r="42" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="9"/>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="9"/>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="9"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B49" s="9"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B50" s="9"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>48</v>
       </c>
@@ -2237,47 +2237,47 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B53" s="9"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C54" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C55" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C56" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C57" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D58" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
         <v>57</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
         <v>59</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
         <v>61</v>
       </c>
@@ -2301,12 +2301,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="16" t="s">
         <v>64</v>
       </c>
@@ -2327,14 +2327,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>70</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>72</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -2395,13 +2395,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2554,9 +2554,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
     </row>
   </sheetData>
@@ -2568,11 +2568,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D486160A-33BA-4485-A4A1-9076EE5057D7}">
   <dimension ref="B2:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="67.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
@@ -2585,12 +2585,12 @@
     <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>95</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>1</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30">
+    <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -2699,115 +2699,115 @@
         <v>115</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="H11" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="2:11" ht="30">
+    <row r="12" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>5</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>6</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="G15" t="s">
         <v>131</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
         <v>132</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>133</v>
       </c>
-      <c r="G15" t="s">
+      <c r="J15" t="s">
         <v>134</v>
       </c>
-      <c r="H15" t="s">
+      <c r="K15" t="s">
         <v>135</v>
       </c>
-      <c r="I15" t="s">
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>136</v>
       </c>
-      <c r="J15" t="s">
+      <c r="C19" t="s">
         <v>137</v>
       </c>
-      <c r="K15" t="s">
+      <c r="E19" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" t="s">
+      <c r="F19" t="s">
         <v>139</v>
       </c>
-      <c r="C19" t="s">
+      <c r="G19" t="s">
         <v>140</v>
-      </c>
-      <c r="E19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2823,29 +2823,29 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="5:8">
+    <row r="2" spans="5:8" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="5:8">
-      <c r="F4" t="s">
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>145</v>
-      </c>
-      <c r="H4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="5:8">
-      <c r="F6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="5:8">
-      <c r="E7" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3104,15 +3104,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -3122,14 +3113,50 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F098F3A-65A4-45F6-BD22-0269253D4075}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F098F3A-65A4-45F6-BD22-0269253D4075}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="90557601-5fe2-4f1f-8c2d-d77dc9e2827d"/>
+    <ds:schemaRef ds:uri="2bf0fcc5-c6e5-4ae9-8d31-e0ef0743f2c2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA0363-1E6B-46B4-9092-70C2D79BA93D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E776AEDC-D6EB-4AD2-9619-D13B42F98854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="90557601-5fe2-4f1f-8c2d-d77dc9e2827d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E776AEDC-D6EB-4AD2-9619-D13B42F98854}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0EA0363-1E6B-46B4-9092-70C2D79BA93D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>